<commit_message>
update alpha effect (~2021/12/31)
</commit_message>
<xml_diff>
--- a/data/covid19/alpha_delta_effect.xlsx
+++ b/data/covid19/alpha_delta_effect.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yjlee/repos/COVID19_SeoulGyeonggi/data/vaccine/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iyunjeong/repos/COVID19_SeoulGyeonggi/data/covid19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE2E1CA-0000-B441-9E6B-E634BB6DFD8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C89DF964-2DAC-944F-933A-CAFD17E68090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="15140" windowHeight="13380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,651 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="231">
-  <si>
-    <t>2021.03.05</t>
-  </si>
-  <si>
-    <t>2021.03.17</t>
-  </si>
-  <si>
-    <t>2021.04.14</t>
-  </si>
-  <si>
-    <t>2021.04.12</t>
-  </si>
-  <si>
-    <t>2021.03.18</t>
-  </si>
-  <si>
-    <t>2021.03.03</t>
-  </si>
-  <si>
-    <t>2021.03.04</t>
-  </si>
-  <si>
-    <t>2021.03.08</t>
-  </si>
-  <si>
-    <t>2021.03.16</t>
-  </si>
-  <si>
-    <t>2021.03.12</t>
-  </si>
-  <si>
-    <t>2021.03.07</t>
-  </si>
-  <si>
-    <t>2021.03.14</t>
-  </si>
-  <si>
-    <t>2021.03.01</t>
-  </si>
-  <si>
-    <t>2021.03.25</t>
-  </si>
-  <si>
-    <t>2021.03.09</t>
-  </si>
-  <si>
-    <t>2021.03.21</t>
-  </si>
-  <si>
-    <t>2021.03.11</t>
-  </si>
-  <si>
-    <t>2021.04.03</t>
-  </si>
-  <si>
-    <t>2021.03.19</t>
-  </si>
-  <si>
-    <t>2021.03.02</t>
-  </si>
-  <si>
-    <t>2021.03.28</t>
-  </si>
-  <si>
-    <t>2021.03.23</t>
-  </si>
-  <si>
-    <t>2021.04.11</t>
-  </si>
-  <si>
-    <t>2021.04.05</t>
-  </si>
-  <si>
-    <t>2021.04.10</t>
-  </si>
-  <si>
-    <t>2021.03.06</t>
-  </si>
-  <si>
-    <t>2021.03.13</t>
-  </si>
-  <si>
-    <t>2021.04.04</t>
-  </si>
-  <si>
-    <t>2021.08.28</t>
-  </si>
-  <si>
-    <t>2021.08.26</t>
-  </si>
-  <si>
-    <t>2021.03.31</t>
-  </si>
-  <si>
-    <t>2021.08.29</t>
-  </si>
-  <si>
-    <t>2021.03.15</t>
-  </si>
-  <si>
-    <t>2021.03.29</t>
-  </si>
-  <si>
-    <t>2021.08.24</t>
-  </si>
-  <si>
-    <t>2021.03.22</t>
-  </si>
-  <si>
-    <t>2021.03.24</t>
-  </si>
-  <si>
-    <t>2021.08.27</t>
-  </si>
-  <si>
-    <t>2021.08.25</t>
-  </si>
-  <si>
-    <t>2021.03.10</t>
-  </si>
-  <si>
-    <t>2021.03.20</t>
-  </si>
-  <si>
-    <t>2021.03.27</t>
-  </si>
-  <si>
-    <t>2021.03.30</t>
-  </si>
-  <si>
-    <t>2021.09.01</t>
-  </si>
-  <si>
-    <t>2021.09.27</t>
-  </si>
-  <si>
-    <t>2021.09.22</t>
-  </si>
-  <si>
-    <t>2021.09.26</t>
-  </si>
-  <si>
-    <t>2021.04.02</t>
-  </si>
-  <si>
-    <t>2021.09.17</t>
-  </si>
-  <si>
-    <t>2021.08.30</t>
-  </si>
-  <si>
-    <t>2021.09.28</t>
-  </si>
-  <si>
-    <t>2021.09.21</t>
-  </si>
-  <si>
-    <t>2021.03.26</t>
-  </si>
-  <si>
-    <t>2021.09.18</t>
-  </si>
-  <si>
-    <t>2021.09.25</t>
-  </si>
-  <si>
-    <t>2021.04.01</t>
-  </si>
-  <si>
-    <t>2021.08.31</t>
-  </si>
-  <si>
-    <t>2021.09.24</t>
-  </si>
-  <si>
-    <t>2021.09.20</t>
-  </si>
-  <si>
-    <t>2021.09.23</t>
-  </si>
-  <si>
-    <t>2021.09.05</t>
-  </si>
-  <si>
-    <t>2021.09.08</t>
-  </si>
-  <si>
-    <t>2021.09.07</t>
-  </si>
-  <si>
-    <t>2021.09.29</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>date/effect</t>
-  </si>
-  <si>
-    <t>2021.09.09</t>
-  </si>
-  <si>
-    <t>2021.09.06</t>
-  </si>
-  <si>
-    <t>2021.09.19</t>
-  </si>
-  <si>
-    <t>2021.04.09</t>
-  </si>
-  <si>
-    <t>2021.04.19</t>
-  </si>
-  <si>
-    <t>2021.04.15</t>
-  </si>
-  <si>
-    <t>2021.04.08</t>
-  </si>
-  <si>
-    <t>2021.04.13</t>
-  </si>
-  <si>
-    <t>2021.04.22</t>
-  </si>
-  <si>
-    <t>2021.04.18</t>
-  </si>
-  <si>
-    <t>2021.04.16</t>
-  </si>
-  <si>
-    <t>2021.04.06</t>
-  </si>
-  <si>
-    <t>2021.04.24</t>
-  </si>
-  <si>
-    <t>2021.04.07</t>
-  </si>
-  <si>
-    <t>2021.06.20</t>
-  </si>
-  <si>
-    <t>2021.06.10</t>
-  </si>
-  <si>
-    <t>2021.06.17</t>
-  </si>
-  <si>
-    <t>2021.06.18</t>
-  </si>
-  <si>
-    <t>2021.05.28</t>
-  </si>
-  <si>
-    <t>2021.06.12</t>
-  </si>
-  <si>
-    <t>2021.06.11</t>
-  </si>
-  <si>
-    <t>2021.06.19</t>
-  </si>
-  <si>
-    <t>2021.06.14</t>
-  </si>
-  <si>
-    <t>2021.06.13</t>
-  </si>
-  <si>
-    <t>2021.06.16</t>
-  </si>
-  <si>
-    <t>2021.06.15</t>
-  </si>
-  <si>
-    <t>2021.06.08</t>
-  </si>
-  <si>
-    <t>2021.06.22</t>
-  </si>
-  <si>
-    <t>2021.06.09</t>
-  </si>
-  <si>
-    <t>2021.06.21</t>
-  </si>
-  <si>
-    <t>2021.06.29</t>
-  </si>
-  <si>
-    <t>2021.07.05</t>
-  </si>
-  <si>
-    <t>2021.07.06</t>
-  </si>
-  <si>
-    <t>2021.07.03</t>
-  </si>
-  <si>
-    <t>2021.07.01</t>
-  </si>
-  <si>
-    <t>2021.06.24</t>
-  </si>
-  <si>
-    <t>2021.06.28</t>
-  </si>
-  <si>
-    <t>2021.06.07</t>
-  </si>
-  <si>
-    <t>2021.07.07</t>
-  </si>
-  <si>
-    <t>2021.06.23</t>
-  </si>
-  <si>
-    <t>2021.07.08</t>
-  </si>
-  <si>
-    <t>2021.06.30</t>
-  </si>
-  <si>
-    <t>2021.06.25</t>
-  </si>
-  <si>
-    <t>2021.07.04</t>
-  </si>
-  <si>
-    <t>2021.06.26</t>
-  </si>
-  <si>
-    <t>2021.06.27</t>
-  </si>
-  <si>
-    <t>2021.07.18</t>
-  </si>
-  <si>
-    <t>2021.07.10</t>
-  </si>
-  <si>
-    <t>2021.07.21</t>
-  </si>
-  <si>
-    <t>2021.07.19</t>
-  </si>
-  <si>
-    <t>2021.07.20</t>
-  </si>
-  <si>
-    <t>2021.07.23</t>
-  </si>
-  <si>
-    <t>2021.07.02</t>
-  </si>
-  <si>
-    <t>2021.07.12</t>
-  </si>
-  <si>
-    <t>2021.07.09</t>
-  </si>
-  <si>
-    <t>2021.07.11</t>
-  </si>
-  <si>
-    <t>2021.07.15</t>
-  </si>
-  <si>
-    <t>2021.07.17</t>
-  </si>
-  <si>
-    <t>2021.07.22</t>
-  </si>
-  <si>
-    <t>2021.07.16</t>
-  </si>
-  <si>
-    <t>2021.07.13</t>
-  </si>
-  <si>
-    <t>2021.07.14</t>
-  </si>
-  <si>
-    <t>2021.04.21</t>
-  </si>
-  <si>
-    <t>2021.04.20</t>
-  </si>
-  <si>
-    <t>2021.04.17</t>
-  </si>
-  <si>
-    <t>2021.04.23</t>
-  </si>
-  <si>
-    <t>2021.07.24</t>
-  </si>
-  <si>
-    <t>2021.08.05</t>
-  </si>
-  <si>
-    <t>2021.09.16</t>
-  </si>
-  <si>
-    <t>2021.09.13</t>
-  </si>
-  <si>
-    <t>2021.09.15</t>
-  </si>
-  <si>
-    <t>2021.09.12</t>
-  </si>
-  <si>
-    <t>2021.08.08</t>
-  </si>
-  <si>
-    <t>2021.08.02</t>
-  </si>
-  <si>
-    <t>2021.09.02</t>
-  </si>
-  <si>
-    <t>2021.09.03</t>
-  </si>
-  <si>
-    <t>2021.09.14</t>
-  </si>
-  <si>
-    <t>2021.09.10</t>
-  </si>
-  <si>
-    <t>2021.07.25</t>
-  </si>
-  <si>
-    <t>2021.08.04</t>
-  </si>
-  <si>
-    <t>2021.09.30</t>
-  </si>
-  <si>
-    <t>2021.08.11</t>
-  </si>
-  <si>
-    <t>2021.09.11</t>
-  </si>
-  <si>
-    <t>2021.08.16</t>
-  </si>
-  <si>
-    <t>2021.08.09</t>
-  </si>
-  <si>
-    <t>2021.08.12</t>
-  </si>
-  <si>
-    <t>2021.09.04</t>
-  </si>
-  <si>
-    <t>2021.08.06</t>
-  </si>
-  <si>
-    <t>2021.08.17</t>
-  </si>
-  <si>
-    <t>2021.08.22</t>
-  </si>
-  <si>
-    <t>2021.08.14</t>
-  </si>
-  <si>
-    <t>2021.08.03</t>
-  </si>
-  <si>
-    <t>2021.07.27</t>
-  </si>
-  <si>
-    <t>2021.08.20</t>
-  </si>
-  <si>
-    <t>2021.08.19</t>
-  </si>
-  <si>
-    <t>2021.08.23</t>
-  </si>
-  <si>
-    <t>2021.07.30</t>
-  </si>
-  <si>
-    <t>2021.08.07</t>
-  </si>
-  <si>
-    <t>2021.08.15</t>
-  </si>
-  <si>
-    <t>2021.08.18</t>
-  </si>
-  <si>
-    <t>2021.08.10</t>
-  </si>
-  <si>
-    <t>2021.08.13</t>
-  </si>
-  <si>
-    <t>2021.08.21</t>
-  </si>
-  <si>
-    <t>2021.05.04</t>
-  </si>
-  <si>
-    <t>2021.04.26</t>
-  </si>
-  <si>
-    <t>2021.04.30</t>
-  </si>
-  <si>
-    <t>2021.05.03</t>
-  </si>
-  <si>
-    <t>2021.05.16</t>
-  </si>
-  <si>
-    <t>2021.04.27</t>
-  </si>
-  <si>
-    <t>2021.05.01</t>
-  </si>
-  <si>
-    <t>2021.07.29</t>
-  </si>
-  <si>
-    <t>2021.07.28</t>
-  </si>
-  <si>
-    <t>2021.08.01</t>
-  </si>
-  <si>
-    <t>2021.07.31</t>
-  </si>
-  <si>
-    <t>2021.04.25</t>
-  </si>
-  <si>
-    <t>2021.04.29</t>
-  </si>
-  <si>
-    <t>2021.04.28</t>
-  </si>
-  <si>
-    <t>2021.07.26</t>
-  </si>
-  <si>
-    <t>2021.05.02</t>
-  </si>
-  <si>
-    <t>2021.05.05</t>
-  </si>
-  <si>
-    <t>2021.05.31</t>
-  </si>
-  <si>
-    <t>2021.05.19</t>
-  </si>
-  <si>
-    <t>2021.05.06</t>
-  </si>
-  <si>
-    <t>2021.05.09</t>
-  </si>
-  <si>
-    <t>2021.05.14</t>
-  </si>
-  <si>
-    <t>2021.05.21</t>
-  </si>
-  <si>
-    <t>2021.05.17</t>
-  </si>
-  <si>
-    <t>2021.05.10</t>
-  </si>
-  <si>
-    <t>2021.05.07</t>
-  </si>
-  <si>
-    <t>2021.05.08</t>
-  </si>
-  <si>
-    <t>2021.05.15</t>
-  </si>
-  <si>
-    <t>2021.05.13</t>
-  </si>
-  <si>
-    <t>2021.05.20</t>
-  </si>
-  <si>
-    <t>2021.05.18</t>
-  </si>
-  <si>
-    <t>2021.05.11</t>
-  </si>
-  <si>
-    <t>2021.05.12</t>
-  </si>
-  <si>
-    <t>2021.05.29</t>
-  </si>
-  <si>
-    <t>2021.05.27</t>
-  </si>
-  <si>
-    <t>2021.05.26</t>
-  </si>
-  <si>
-    <t>2021.05.23</t>
-  </si>
-  <si>
-    <t>2021.05.22</t>
-  </si>
-  <si>
-    <t>2021.05.25</t>
-  </si>
-  <si>
-    <t>2021.06.06</t>
-  </si>
-  <si>
-    <t>2021.05.30</t>
-  </si>
-  <si>
-    <t>2021.06.02</t>
-  </si>
-  <si>
-    <t>2021.05.24</t>
-  </si>
-  <si>
-    <t>2021.06.03</t>
-  </si>
-  <si>
-    <t>2021.06.04</t>
-  </si>
-  <si>
-    <t>2021.06.05</t>
-  </si>
-  <si>
-    <t>2021.06.01</t>
   </si>
   <si>
     <t>alpha</t>
@@ -672,58 +30,27 @@
   <si>
     <t>delta</t>
   </si>
-  <si>
-    <t>2021.02.15</t>
-  </si>
-  <si>
-    <t>2021.02.28</t>
-  </si>
-  <si>
-    <t>2021.02.16</t>
-  </si>
-  <si>
-    <t>2021.02.19</t>
-  </si>
-  <si>
-    <t>2021.02.17</t>
-  </si>
-  <si>
-    <t>2021.02.23</t>
-  </si>
-  <si>
-    <t>2021.02.21</t>
-  </si>
-  <si>
-    <t>2021.02.22</t>
-  </si>
-  <si>
-    <t>2021.02.18</t>
-  </si>
-  <si>
-    <t>2021.02.20</t>
-  </si>
-  <si>
-    <t>2021.02.27</t>
-  </si>
-  <si>
-    <t>2021.02.24</t>
-  </si>
-  <si>
-    <t>2021.02.25</t>
-  </si>
-  <si>
-    <t>2021.02.26</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="맑은 고딕"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
     </font>
   </fonts>
   <fills count="2">
@@ -748,11 +75,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -938,7 +271,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="Normal Style 1 - Accent 1" defaultPivotStyle="Light Style 1 - Accent 1">
-    <tableStyle name="Normal Style 1 - Accent 1" pivot="0" count="9" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="Normal Style 1 - Accent 1" pivot="0" count="7" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="13"/>
       <tableStyleElement type="headerRow" dxfId="12"/>
       <tableStyleElement type="totalRow" dxfId="11"/>
@@ -947,7 +280,7 @@
       <tableStyleElement type="firstRowStripe" dxfId="8"/>
       <tableStyleElement type="firstColumnStripe" dxfId="7"/>
     </tableStyle>
-    <tableStyle name="Light Style 1 - Accent 1" table="0" count="8" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
+    <tableStyle name="Light Style 1 - Accent 1" table="0" count="7" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
       <tableStyleElement type="wholeTable" dxfId="6"/>
       <tableStyleElement type="headerRow" dxfId="5"/>
       <tableStyleElement type="totalRow" dxfId="4"/>
@@ -1224,33 +557,33 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C229"/>
+  <dimension ref="A1:C321"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="A77" sqref="A77:XFD77"/>
+    <sheetView tabSelected="1" topLeftCell="A297" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="B226" sqref="B226:C321"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>215</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>216</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>217</v>
+      <c r="A2" s="2">
+        <v>44242</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1260,8 +593,8 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>219</v>
+      <c r="A3" s="3">
+        <v>44243</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1271,8 +604,8 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>221</v>
+      <c r="A4" s="2">
+        <v>44244</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1282,8 +615,8 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>225</v>
+      <c r="A5" s="3">
+        <v>44245</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -1293,8 +626,8 @@
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>220</v>
+      <c r="A6" s="2">
+        <v>44246</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1304,8 +637,8 @@
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>226</v>
+      <c r="A7" s="3">
+        <v>44247</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -1315,8 +648,8 @@
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>223</v>
+      <c r="A8" s="2">
+        <v>44248</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -1326,8 +659,8 @@
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>224</v>
+      <c r="A9" s="3">
+        <v>44249</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1337,8 +670,8 @@
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>222</v>
+      <c r="A10" s="2">
+        <v>44250</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1348,8 +681,8 @@
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>228</v>
+      <c r="A11" s="3">
+        <v>44251</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1359,8 +692,8 @@
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>229</v>
+      <c r="A12" s="2">
+        <v>44252</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1370,8 +703,8 @@
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>230</v>
+      <c r="A13" s="3">
+        <v>44253</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -1381,8 +714,8 @@
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>227</v>
+      <c r="A14" s="2">
+        <v>44254</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -1392,8 +725,8 @@
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" t="s">
-        <v>218</v>
+      <c r="A15" s="3">
+        <v>44255</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1403,8 +736,8 @@
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="1" t="s">
-        <v>12</v>
+      <c r="A16" s="2">
+        <v>44256</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
@@ -1414,8 +747,8 @@
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="1" t="s">
-        <v>19</v>
+      <c r="A17" s="3">
+        <v>44257</v>
       </c>
       <c r="B17" s="1">
         <v>1</v>
@@ -1425,8 +758,8 @@
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="1" t="s">
-        <v>5</v>
+      <c r="A18" s="2">
+        <v>44258</v>
       </c>
       <c r="B18" s="1">
         <v>1</v>
@@ -1436,8 +769,8 @@
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="1" t="s">
-        <v>6</v>
+      <c r="A19" s="3">
+        <v>44259</v>
       </c>
       <c r="B19" s="1">
         <v>1</v>
@@ -1447,8 +780,8 @@
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="1" t="s">
-        <v>0</v>
+      <c r="A20" s="2">
+        <v>44260</v>
       </c>
       <c r="B20" s="1">
         <v>1</v>
@@ -1458,8 +791,8 @@
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="1" t="s">
-        <v>25</v>
+      <c r="A21" s="3">
+        <v>44261</v>
       </c>
       <c r="B21" s="1">
         <v>1</v>
@@ -1469,8 +802,8 @@
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="1" t="s">
-        <v>10</v>
+      <c r="A22" s="2">
+        <v>44262</v>
       </c>
       <c r="B22" s="1">
         <v>1</v>
@@ -1480,8 +813,8 @@
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="1" t="s">
-        <v>7</v>
+      <c r="A23" s="3">
+        <v>44263</v>
       </c>
       <c r="B23" s="1">
         <v>1</v>
@@ -1491,8 +824,8 @@
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="1" t="s">
-        <v>14</v>
+      <c r="A24" s="2">
+        <v>44264</v>
       </c>
       <c r="B24" s="1">
         <v>1</v>
@@ -1502,8 +835,8 @@
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="1" t="s">
-        <v>39</v>
+      <c r="A25" s="3">
+        <v>44265</v>
       </c>
       <c r="B25" s="1">
         <v>1</v>
@@ -1513,8 +846,8 @@
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="1" t="s">
-        <v>16</v>
+      <c r="A26" s="2">
+        <v>44266</v>
       </c>
       <c r="B26" s="1">
         <v>1</v>
@@ -1524,8 +857,8 @@
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="1" t="s">
-        <v>9</v>
+      <c r="A27" s="3">
+        <v>44267</v>
       </c>
       <c r="B27" s="1">
         <v>1</v>
@@ -1535,8 +868,8 @@
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="1" t="s">
-        <v>26</v>
+      <c r="A28" s="2">
+        <v>44268</v>
       </c>
       <c r="B28" s="1">
         <v>1</v>
@@ -1546,8 +879,8 @@
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="1" t="s">
-        <v>11</v>
+      <c r="A29" s="3">
+        <v>44269</v>
       </c>
       <c r="B29" s="1">
         <v>1</v>
@@ -1557,8 +890,8 @@
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="1" t="s">
-        <v>32</v>
+      <c r="A30" s="2">
+        <v>44270</v>
       </c>
       <c r="B30" s="1">
         <v>1</v>
@@ -1568,8 +901,8 @@
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="1" t="s">
-        <v>8</v>
+      <c r="A31" s="3">
+        <v>44271</v>
       </c>
       <c r="B31" s="1">
         <v>1</v>
@@ -1579,8 +912,8 @@
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="1" t="s">
-        <v>1</v>
+      <c r="A32" s="2">
+        <v>44272</v>
       </c>
       <c r="B32" s="1">
         <v>1</v>
@@ -1590,8 +923,8 @@
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="1" t="s">
-        <v>4</v>
+      <c r="A33" s="3">
+        <v>44273</v>
       </c>
       <c r="B33" s="1">
         <v>1</v>
@@ -1601,8 +934,8 @@
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="1" t="s">
-        <v>18</v>
+      <c r="A34" s="2">
+        <v>44274</v>
       </c>
       <c r="B34" s="1">
         <v>1</v>
@@ -1612,8 +945,8 @@
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="1" t="s">
-        <v>40</v>
+      <c r="A35" s="3">
+        <v>44275</v>
       </c>
       <c r="B35" s="1">
         <v>1</v>
@@ -1623,8 +956,8 @@
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="1" t="s">
-        <v>15</v>
+      <c r="A36" s="2">
+        <v>44276</v>
       </c>
       <c r="B36" s="1">
         <v>1</v>
@@ -1634,8 +967,8 @@
       </c>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="1" t="s">
-        <v>35</v>
+      <c r="A37" s="3">
+        <v>44277</v>
       </c>
       <c r="B37" s="1">
         <v>1</v>
@@ -1645,8 +978,8 @@
       </c>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="1" t="s">
-        <v>21</v>
+      <c r="A38" s="2">
+        <v>44278</v>
       </c>
       <c r="B38" s="1">
         <v>1</v>
@@ -1656,8 +989,8 @@
       </c>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="1" t="s">
-        <v>36</v>
+      <c r="A39" s="3">
+        <v>44279</v>
       </c>
       <c r="B39" s="1">
         <v>1</v>
@@ -1667,8 +1000,8 @@
       </c>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" s="1" t="s">
-        <v>13</v>
+      <c r="A40" s="2">
+        <v>44280</v>
       </c>
       <c r="B40" s="1">
         <v>1</v>
@@ -1678,8 +1011,8 @@
       </c>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="1" t="s">
-        <v>52</v>
+      <c r="A41" s="3">
+        <v>44281</v>
       </c>
       <c r="B41" s="1">
         <v>1</v>
@@ -1689,8 +1022,8 @@
       </c>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="1" t="s">
-        <v>41</v>
+      <c r="A42" s="2">
+        <v>44282</v>
       </c>
       <c r="B42" s="1">
         <v>1</v>
@@ -1700,8 +1033,8 @@
       </c>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" s="1" t="s">
-        <v>20</v>
+      <c r="A43" s="3">
+        <v>44283</v>
       </c>
       <c r="B43" s="1">
         <v>1</v>
@@ -1711,8 +1044,8 @@
       </c>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" s="1" t="s">
-        <v>33</v>
+      <c r="A44" s="2">
+        <v>44284</v>
       </c>
       <c r="B44" s="1">
         <v>1</v>
@@ -1722,8 +1055,8 @@
       </c>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="1" t="s">
-        <v>42</v>
+      <c r="A45" s="3">
+        <v>44285</v>
       </c>
       <c r="B45" s="1">
         <v>1</v>
@@ -1733,8 +1066,8 @@
       </c>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="1" t="s">
-        <v>30</v>
+      <c r="A46" s="2">
+        <v>44286</v>
       </c>
       <c r="B46" s="1">
         <v>1</v>
@@ -1744,8 +1077,8 @@
       </c>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="1" t="s">
-        <v>55</v>
+      <c r="A47" s="3">
+        <v>44287</v>
       </c>
       <c r="B47" s="1">
         <v>1</v>
@@ -1755,8 +1088,8 @@
       </c>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" s="1" t="s">
-        <v>47</v>
+      <c r="A48" s="2">
+        <v>44288</v>
       </c>
       <c r="B48" s="1">
         <v>1</v>
@@ -1766,8 +1099,8 @@
       </c>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="1" t="s">
-        <v>17</v>
+      <c r="A49" s="3">
+        <v>44289</v>
       </c>
       <c r="B49" s="1">
         <v>1</v>
@@ -1777,8 +1110,8 @@
       </c>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="1" t="s">
-        <v>27</v>
+      <c r="A50" s="2">
+        <v>44290</v>
       </c>
       <c r="B50" s="1">
         <v>1</v>
@@ -1788,8 +1121,8 @@
       </c>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="1" t="s">
-        <v>23</v>
+      <c r="A51" s="3">
+        <v>44291</v>
       </c>
       <c r="B51" s="1">
         <v>1</v>
@@ -1799,8 +1132,8 @@
       </c>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="1" t="s">
-        <v>76</v>
+      <c r="A52" s="2">
+        <v>44292</v>
       </c>
       <c r="B52" s="1">
         <v>1</v>
@@ -1810,8 +1143,8 @@
       </c>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="1" t="s">
-        <v>78</v>
+      <c r="A53" s="3">
+        <v>44293</v>
       </c>
       <c r="B53" s="1">
         <v>1</v>
@@ -1821,8 +1154,8 @@
       </c>
     </row>
     <row r="54" spans="1:3">
-      <c r="A54" s="1" t="s">
-        <v>71</v>
+      <c r="A54" s="2">
+        <v>44294</v>
       </c>
       <c r="B54" s="1">
         <v>1</v>
@@ -1832,8 +1165,8 @@
       </c>
     </row>
     <row r="55" spans="1:3">
-      <c r="A55" s="1" t="s">
-        <v>68</v>
+      <c r="A55" s="3">
+        <v>44295</v>
       </c>
       <c r="B55" s="1">
         <v>1</v>
@@ -1843,8 +1176,8 @@
       </c>
     </row>
     <row r="56" spans="1:3">
-      <c r="A56" s="1" t="s">
-        <v>24</v>
+      <c r="A56" s="2">
+        <v>44296</v>
       </c>
       <c r="B56" s="1">
         <v>1</v>
@@ -1854,8 +1187,8 @@
       </c>
     </row>
     <row r="57" spans="1:3">
-      <c r="A57" s="1" t="s">
-        <v>22</v>
+      <c r="A57" s="3">
+        <v>44297</v>
       </c>
       <c r="B57" s="1">
         <v>1</v>
@@ -1865,8 +1198,8 @@
       </c>
     </row>
     <row r="58" spans="1:3">
-      <c r="A58" s="1" t="s">
-        <v>3</v>
+      <c r="A58" s="2">
+        <v>44298</v>
       </c>
       <c r="B58" s="1">
         <v>1</v>
@@ -1876,8 +1209,8 @@
       </c>
     </row>
     <row r="59" spans="1:3">
-      <c r="A59" s="1" t="s">
-        <v>72</v>
+      <c r="A59" s="3">
+        <v>44299</v>
       </c>
       <c r="B59" s="1">
         <v>1</v>
@@ -1887,8 +1220,8 @@
       </c>
     </row>
     <row r="60" spans="1:3">
-      <c r="A60" s="1" t="s">
-        <v>2</v>
+      <c r="A60" s="2">
+        <v>44300</v>
       </c>
       <c r="B60" s="1">
         <v>1</v>
@@ -1898,8 +1231,8 @@
       </c>
     </row>
     <row r="61" spans="1:3">
-      <c r="A61" s="1" t="s">
-        <v>70</v>
+      <c r="A61" s="3">
+        <v>44301</v>
       </c>
       <c r="B61" s="1">
         <v>1</v>
@@ -1909,8 +1242,8 @@
       </c>
     </row>
     <row r="62" spans="1:3">
-      <c r="A62" s="1" t="s">
-        <v>75</v>
+      <c r="A62" s="2">
+        <v>44302</v>
       </c>
       <c r="B62" s="1">
         <v>1</v>
@@ -1920,8 +1253,8 @@
       </c>
     </row>
     <row r="63" spans="1:3">
-      <c r="A63" s="1" t="s">
-        <v>129</v>
+      <c r="A63" s="3">
+        <v>44303</v>
       </c>
       <c r="B63" s="1">
         <v>1</v>
@@ -1931,8 +1264,8 @@
       </c>
     </row>
     <row r="64" spans="1:3">
-      <c r="A64" s="1" t="s">
-        <v>74</v>
+      <c r="A64" s="2">
+        <v>44304</v>
       </c>
       <c r="B64" s="1">
         <v>1</v>
@@ -1942,8 +1275,8 @@
       </c>
     </row>
     <row r="65" spans="1:3">
-      <c r="A65" s="1" t="s">
-        <v>69</v>
+      <c r="A65" s="3">
+        <v>44305</v>
       </c>
       <c r="B65" s="1">
         <v>1</v>
@@ -1953,8 +1286,8 @@
       </c>
     </row>
     <row r="66" spans="1:3">
-      <c r="A66" s="1" t="s">
-        <v>128</v>
+      <c r="A66" s="2">
+        <v>44306</v>
       </c>
       <c r="B66" s="1">
         <v>1</v>
@@ -1964,8 +1297,8 @@
       </c>
     </row>
     <row r="67" spans="1:3">
-      <c r="A67" s="1" t="s">
-        <v>127</v>
+      <c r="A67" s="3">
+        <v>44307</v>
       </c>
       <c r="B67" s="1">
         <v>1</v>
@@ -1975,8 +1308,8 @@
       </c>
     </row>
     <row r="68" spans="1:3">
-      <c r="A68" s="1" t="s">
-        <v>73</v>
+      <c r="A68" s="2">
+        <v>44308</v>
       </c>
       <c r="B68" s="1">
         <v>1</v>
@@ -1986,8 +1319,8 @@
       </c>
     </row>
     <row r="69" spans="1:3">
-      <c r="A69" s="1" t="s">
-        <v>130</v>
+      <c r="A69" s="3">
+        <v>44309</v>
       </c>
       <c r="B69" s="1">
         <v>1</v>
@@ -1997,8 +1330,8 @@
       </c>
     </row>
     <row r="70" spans="1:3">
-      <c r="A70" s="1" t="s">
-        <v>77</v>
+      <c r="A70" s="2">
+        <v>44310</v>
       </c>
       <c r="B70" s="1">
         <v>1</v>
@@ -2008,8 +1341,8 @@
       </c>
     </row>
     <row r="71" spans="1:3">
-      <c r="A71" s="1" t="s">
-        <v>179</v>
+      <c r="A71" s="3">
+        <v>44311</v>
       </c>
       <c r="B71" s="1">
         <v>1</v>
@@ -2019,8 +1352,8 @@
       </c>
     </row>
     <row r="72" spans="1:3">
-      <c r="A72" s="1" t="s">
-        <v>169</v>
+      <c r="A72" s="2">
+        <v>44312</v>
       </c>
       <c r="B72" s="1">
         <v>1</v>
@@ -2030,8 +1363,8 @@
       </c>
     </row>
     <row r="73" spans="1:3">
-      <c r="A73" s="1" t="s">
-        <v>173</v>
+      <c r="A73" s="3">
+        <v>44313</v>
       </c>
       <c r="B73" s="1">
         <v>1</v>
@@ -2041,8 +1374,8 @@
       </c>
     </row>
     <row r="74" spans="1:3">
-      <c r="A74" s="1" t="s">
-        <v>181</v>
+      <c r="A74" s="2">
+        <v>44314</v>
       </c>
       <c r="B74" s="1">
         <v>1</v>
@@ -2052,8 +1385,8 @@
       </c>
     </row>
     <row r="75" spans="1:3">
-      <c r="A75" s="1" t="s">
-        <v>180</v>
+      <c r="A75" s="3">
+        <v>44315</v>
       </c>
       <c r="B75" s="1">
         <v>1</v>
@@ -2063,8 +1396,8 @@
       </c>
     </row>
     <row r="76" spans="1:3">
-      <c r="A76" s="1" t="s">
-        <v>170</v>
+      <c r="A76" s="2">
+        <v>44316</v>
       </c>
       <c r="B76" s="1">
         <v>1</v>
@@ -2074,8 +1407,8 @@
       </c>
     </row>
     <row r="77" spans="1:3">
-      <c r="A77" s="1" t="s">
-        <v>174</v>
+      <c r="A77" s="3">
+        <v>44317</v>
       </c>
       <c r="B77" s="1">
         <v>1</v>
@@ -2085,8 +1418,8 @@
       </c>
     </row>
     <row r="78" spans="1:3">
-      <c r="A78" s="1" t="s">
-        <v>183</v>
+      <c r="A78" s="2">
+        <v>44318</v>
       </c>
       <c r="B78" s="1">
         <v>1</v>
@@ -2096,8 +1429,8 @@
       </c>
     </row>
     <row r="79" spans="1:3">
-      <c r="A79" s="1" t="s">
-        <v>171</v>
+      <c r="A79" s="3">
+        <v>44319</v>
       </c>
       <c r="B79" s="1">
         <v>1</v>
@@ -2107,8 +1440,8 @@
       </c>
     </row>
     <row r="80" spans="1:3">
-      <c r="A80" s="1" t="s">
-        <v>168</v>
+      <c r="A80" s="2">
+        <v>44320</v>
       </c>
       <c r="B80" s="1">
         <v>1</v>
@@ -2118,8 +1451,8 @@
       </c>
     </row>
     <row r="81" spans="1:3">
-      <c r="A81" s="1" t="s">
-        <v>184</v>
+      <c r="A81" s="3">
+        <v>44321</v>
       </c>
       <c r="B81" s="1">
         <v>1</v>
@@ -2129,8 +1462,8 @@
       </c>
     </row>
     <row r="82" spans="1:3">
-      <c r="A82" s="1" t="s">
-        <v>187</v>
+      <c r="A82" s="2">
+        <v>44322</v>
       </c>
       <c r="B82" s="1">
         <v>1</v>
@@ -2140,8 +1473,8 @@
       </c>
     </row>
     <row r="83" spans="1:3">
-      <c r="A83" s="1" t="s">
-        <v>193</v>
+      <c r="A83" s="3">
+        <v>44323</v>
       </c>
       <c r="B83" s="1">
         <v>1</v>
@@ -2151,8 +1484,8 @@
       </c>
     </row>
     <row r="84" spans="1:3">
-      <c r="A84" s="1" t="s">
-        <v>194</v>
+      <c r="A84" s="2">
+        <v>44324</v>
       </c>
       <c r="B84" s="1">
         <v>1</v>
@@ -2162,8 +1495,8 @@
       </c>
     </row>
     <row r="85" spans="1:3">
-      <c r="A85" s="1" t="s">
-        <v>188</v>
+      <c r="A85" s="3">
+        <v>44325</v>
       </c>
       <c r="B85" s="1">
         <v>1</v>
@@ -2173,8 +1506,8 @@
       </c>
     </row>
     <row r="86" spans="1:3">
-      <c r="A86" s="1" t="s">
-        <v>192</v>
+      <c r="A86" s="2">
+        <v>44326</v>
       </c>
       <c r="B86" s="1">
         <v>1</v>
@@ -2184,8 +1517,8 @@
       </c>
     </row>
     <row r="87" spans="1:3">
-      <c r="A87" s="1" t="s">
-        <v>199</v>
+      <c r="A87" s="3">
+        <v>44327</v>
       </c>
       <c r="B87" s="1">
         <v>1</v>
@@ -2195,8 +1528,8 @@
       </c>
     </row>
     <row r="88" spans="1:3">
-      <c r="A88" s="1" t="s">
-        <v>200</v>
+      <c r="A88" s="2">
+        <v>44328</v>
       </c>
       <c r="B88" s="1">
         <v>1</v>
@@ -2206,8 +1539,8 @@
       </c>
     </row>
     <row r="89" spans="1:3">
-      <c r="A89" s="1" t="s">
-        <v>196</v>
+      <c r="A89" s="3">
+        <v>44329</v>
       </c>
       <c r="B89" s="1">
         <v>1</v>
@@ -2217,8 +1550,8 @@
       </c>
     </row>
     <row r="90" spans="1:3">
-      <c r="A90" s="1" t="s">
-        <v>189</v>
+      <c r="A90" s="2">
+        <v>44330</v>
       </c>
       <c r="B90" s="1">
         <v>1</v>
@@ -2228,8 +1561,8 @@
       </c>
     </row>
     <row r="91" spans="1:3">
-      <c r="A91" s="1" t="s">
-        <v>195</v>
+      <c r="A91" s="3">
+        <v>44331</v>
       </c>
       <c r="B91" s="1">
         <v>1</v>
@@ -2239,8 +1572,8 @@
       </c>
     </row>
     <row r="92" spans="1:3">
-      <c r="A92" s="1" t="s">
-        <v>172</v>
+      <c r="A92" s="2">
+        <v>44332</v>
       </c>
       <c r="B92" s="1">
         <v>1</v>
@@ -2250,8 +1583,8 @@
       </c>
     </row>
     <row r="93" spans="1:3">
-      <c r="A93" s="1" t="s">
-        <v>191</v>
+      <c r="A93" s="3">
+        <v>44333</v>
       </c>
       <c r="B93" s="1">
         <v>1</v>
@@ -2261,8 +1594,8 @@
       </c>
     </row>
     <row r="94" spans="1:3">
-      <c r="A94" s="1" t="s">
-        <v>198</v>
+      <c r="A94" s="2">
+        <v>44334</v>
       </c>
       <c r="B94" s="1">
         <v>1</v>
@@ -2272,8 +1605,8 @@
       </c>
     </row>
     <row r="95" spans="1:3">
-      <c r="A95" s="1" t="s">
-        <v>186</v>
+      <c r="A95" s="3">
+        <v>44335</v>
       </c>
       <c r="B95" s="1">
         <v>1</v>
@@ -2283,8 +1616,8 @@
       </c>
     </row>
     <row r="96" spans="1:3">
-      <c r="A96" s="1" t="s">
-        <v>197</v>
+      <c r="A96" s="2">
+        <v>44336</v>
       </c>
       <c r="B96" s="1">
         <v>1</v>
@@ -2294,8 +1627,8 @@
       </c>
     </row>
     <row r="97" spans="1:3">
-      <c r="A97" s="1" t="s">
-        <v>190</v>
+      <c r="A97" s="3">
+        <v>44337</v>
       </c>
       <c r="B97" s="1">
         <v>1</v>
@@ -2305,8 +1638,8 @@
       </c>
     </row>
     <row r="98" spans="1:3">
-      <c r="A98" s="1" t="s">
-        <v>205</v>
+      <c r="A98" s="2">
+        <v>44338</v>
       </c>
       <c r="B98" s="1">
         <v>1</v>
@@ -2316,8 +1649,8 @@
       </c>
     </row>
     <row r="99" spans="1:3">
-      <c r="A99" s="1" t="s">
-        <v>204</v>
+      <c r="A99" s="3">
+        <v>44339</v>
       </c>
       <c r="B99" s="1">
         <v>1</v>
@@ -2327,8 +1660,8 @@
       </c>
     </row>
     <row r="100" spans="1:3">
-      <c r="A100" s="1" t="s">
-        <v>210</v>
+      <c r="A100" s="2">
+        <v>44340</v>
       </c>
       <c r="B100" s="1">
         <v>1</v>
@@ -2338,8 +1671,8 @@
       </c>
     </row>
     <row r="101" spans="1:3">
-      <c r="A101" s="1" t="s">
-        <v>206</v>
+      <c r="A101" s="3">
+        <v>44341</v>
       </c>
       <c r="B101" s="1">
         <v>1</v>
@@ -2349,8 +1682,8 @@
       </c>
     </row>
     <row r="102" spans="1:3">
-      <c r="A102" s="1" t="s">
-        <v>203</v>
+      <c r="A102" s="2">
+        <v>44342</v>
       </c>
       <c r="B102" s="1">
         <v>1</v>
@@ -2360,8 +1693,8 @@
       </c>
     </row>
     <row r="103" spans="1:3">
-      <c r="A103" s="1" t="s">
-        <v>202</v>
+      <c r="A103" s="3">
+        <v>44343</v>
       </c>
       <c r="B103" s="1">
         <v>1</v>
@@ -2371,8 +1704,8 @@
       </c>
     </row>
     <row r="104" spans="1:3">
-      <c r="A104" s="1" t="s">
-        <v>83</v>
+      <c r="A104" s="2">
+        <v>44344</v>
       </c>
       <c r="B104" s="1">
         <v>1</v>
@@ -2382,8 +1715,8 @@
       </c>
     </row>
     <row r="105" spans="1:3">
-      <c r="A105" s="1" t="s">
-        <v>201</v>
+      <c r="A105" s="3">
+        <v>44345</v>
       </c>
       <c r="B105" s="1">
         <v>1</v>
@@ -2393,8 +1726,8 @@
       </c>
     </row>
     <row r="106" spans="1:3">
-      <c r="A106" s="1" t="s">
-        <v>208</v>
+      <c r="A106" s="2">
+        <v>44346</v>
       </c>
       <c r="B106" s="1">
         <v>1</v>
@@ -2404,8 +1737,8 @@
       </c>
     </row>
     <row r="107" spans="1:3">
-      <c r="A107" s="1" t="s">
-        <v>185</v>
+      <c r="A107" s="3">
+        <v>44347</v>
       </c>
       <c r="B107" s="1">
         <v>1</v>
@@ -2415,8 +1748,8 @@
       </c>
     </row>
     <row r="108" spans="1:3">
-      <c r="A108" s="1" t="s">
-        <v>214</v>
+      <c r="A108" s="2">
+        <v>44348</v>
       </c>
       <c r="B108" s="1">
         <v>0.95299999999999996</v>
@@ -2426,8 +1759,8 @@
       </c>
     </row>
     <row r="109" spans="1:3">
-      <c r="A109" s="1" t="s">
-        <v>209</v>
+      <c r="A109" s="3">
+        <v>44349</v>
       </c>
       <c r="B109" s="1">
         <v>0.95299999999999996</v>
@@ -2437,8 +1770,8 @@
       </c>
     </row>
     <row r="110" spans="1:3">
-      <c r="A110" s="1" t="s">
-        <v>211</v>
+      <c r="A110" s="2">
+        <v>44350</v>
       </c>
       <c r="B110" s="1">
         <v>0.95299999999999996</v>
@@ -2448,8 +1781,8 @@
       </c>
     </row>
     <row r="111" spans="1:3">
-      <c r="A111" s="1" t="s">
-        <v>212</v>
+      <c r="A111" s="3">
+        <v>44351</v>
       </c>
       <c r="B111" s="1">
         <v>0.95299999999999996</v>
@@ -2459,8 +1792,8 @@
       </c>
     </row>
     <row r="112" spans="1:3">
-      <c r="A112" s="1" t="s">
-        <v>213</v>
+      <c r="A112" s="2">
+        <v>44352</v>
       </c>
       <c r="B112" s="1">
         <v>0.95299999999999996</v>
@@ -2470,8 +1803,8 @@
       </c>
     </row>
     <row r="113" spans="1:3">
-      <c r="A113" s="1" t="s">
-        <v>207</v>
+      <c r="A113" s="3">
+        <v>44353</v>
       </c>
       <c r="B113" s="1">
         <v>0.97199999999999998</v>
@@ -2481,8 +1814,8 @@
       </c>
     </row>
     <row r="114" spans="1:3">
-      <c r="A114" s="1" t="s">
-        <v>102</v>
+      <c r="A114" s="2">
+        <v>44354</v>
       </c>
       <c r="B114" s="1">
         <v>0.97199999999999998</v>
@@ -2492,8 +1825,8 @@
       </c>
     </row>
     <row r="115" spans="1:3">
-      <c r="A115" s="1" t="s">
-        <v>91</v>
+      <c r="A115" s="3">
+        <v>44355</v>
       </c>
       <c r="B115" s="1">
         <v>0.97199999999999998</v>
@@ -2503,8 +1836,8 @@
       </c>
     </row>
     <row r="116" spans="1:3">
-      <c r="A116" s="1" t="s">
-        <v>93</v>
+      <c r="A116" s="2">
+        <v>44356</v>
       </c>
       <c r="B116" s="1">
         <v>0.97199999999999998</v>
@@ -2514,8 +1847,8 @@
       </c>
     </row>
     <row r="117" spans="1:3">
-      <c r="A117" s="1" t="s">
-        <v>80</v>
+      <c r="A117" s="3">
+        <v>44357</v>
       </c>
       <c r="B117" s="1">
         <v>0.97199999999999998</v>
@@ -2525,8 +1858,8 @@
       </c>
     </row>
     <row r="118" spans="1:3">
-      <c r="A118" s="1" t="s">
-        <v>85</v>
+      <c r="A118" s="2">
+        <v>44358</v>
       </c>
       <c r="B118" s="1">
         <v>0.97199999999999998</v>
@@ -2536,8 +1869,8 @@
       </c>
     </row>
     <row r="119" spans="1:3">
-      <c r="A119" s="1" t="s">
-        <v>84</v>
+      <c r="A119" s="3">
+        <v>44359</v>
       </c>
       <c r="B119" s="1">
         <v>0.97199999999999998</v>
@@ -2547,8 +1880,8 @@
       </c>
     </row>
     <row r="120" spans="1:3">
-      <c r="A120" s="1" t="s">
-        <v>88</v>
+      <c r="A120" s="2">
+        <v>44360</v>
       </c>
       <c r="B120" s="1">
         <v>0.96399999999999997</v>
@@ -2558,8 +1891,8 @@
       </c>
     </row>
     <row r="121" spans="1:3">
-      <c r="A121" s="1" t="s">
-        <v>87</v>
+      <c r="A121" s="3">
+        <v>44361</v>
       </c>
       <c r="B121" s="1">
         <v>0.96399999999999997</v>
@@ -2569,8 +1902,8 @@
       </c>
     </row>
     <row r="122" spans="1:3">
-      <c r="A122" s="1" t="s">
-        <v>90</v>
+      <c r="A122" s="2">
+        <v>44362</v>
       </c>
       <c r="B122" s="1">
         <v>0.96399999999999997</v>
@@ -2580,8 +1913,8 @@
       </c>
     </row>
     <row r="123" spans="1:3">
-      <c r="A123" s="1" t="s">
-        <v>89</v>
+      <c r="A123" s="3">
+        <v>44363</v>
       </c>
       <c r="B123" s="1">
         <v>0.96399999999999997</v>
@@ -2591,8 +1924,8 @@
       </c>
     </row>
     <row r="124" spans="1:3">
-      <c r="A124" s="1" t="s">
-        <v>81</v>
+      <c r="A124" s="2">
+        <v>44364</v>
       </c>
       <c r="B124" s="1">
         <v>0.96399999999999997</v>
@@ -2602,8 +1935,8 @@
       </c>
     </row>
     <row r="125" spans="1:3">
-      <c r="A125" s="1" t="s">
-        <v>82</v>
+      <c r="A125" s="3">
+        <v>44365</v>
       </c>
       <c r="B125" s="1">
         <v>0.96399999999999997</v>
@@ -2613,8 +1946,8 @@
       </c>
     </row>
     <row r="126" spans="1:3">
-      <c r="A126" s="1" t="s">
-        <v>86</v>
+      <c r="A126" s="2">
+        <v>44366</v>
       </c>
       <c r="B126" s="1">
         <v>0.96399999999999997</v>
@@ -2624,8 +1957,8 @@
       </c>
     </row>
     <row r="127" spans="1:3">
-      <c r="A127" s="1" t="s">
-        <v>79</v>
+      <c r="A127" s="3">
+        <v>44367</v>
       </c>
       <c r="B127" s="1">
         <v>0.95499999999999996</v>
@@ -2635,8 +1968,8 @@
       </c>
     </row>
     <row r="128" spans="1:3">
-      <c r="A128" s="1" t="s">
-        <v>94</v>
+      <c r="A128" s="2">
+        <v>44368</v>
       </c>
       <c r="B128" s="1">
         <v>0.95499999999999996</v>
@@ -2646,8 +1979,8 @@
       </c>
     </row>
     <row r="129" spans="1:3">
-      <c r="A129" s="1" t="s">
-        <v>92</v>
+      <c r="A129" s="3">
+        <v>44369</v>
       </c>
       <c r="B129" s="1">
         <v>0.95499999999999996</v>
@@ -2657,8 +1990,8 @@
       </c>
     </row>
     <row r="130" spans="1:3">
-      <c r="A130" s="1" t="s">
-        <v>104</v>
+      <c r="A130" s="2">
+        <v>44370</v>
       </c>
       <c r="B130" s="1">
         <v>0.95499999999999996</v>
@@ -2668,8 +2001,8 @@
       </c>
     </row>
     <row r="131" spans="1:3">
-      <c r="A131" s="1" t="s">
-        <v>100</v>
+      <c r="A131" s="3">
+        <v>44371</v>
       </c>
       <c r="B131" s="1">
         <v>0.95499999999999996</v>
@@ -2679,8 +2012,8 @@
       </c>
     </row>
     <row r="132" spans="1:3">
-      <c r="A132" s="1" t="s">
-        <v>107</v>
+      <c r="A132" s="2">
+        <v>44372</v>
       </c>
       <c r="B132" s="1">
         <v>0.95499999999999996</v>
@@ -2690,8 +2023,8 @@
       </c>
     </row>
     <row r="133" spans="1:3">
-      <c r="A133" s="1" t="s">
-        <v>109</v>
+      <c r="A133" s="3">
+        <v>44373</v>
       </c>
       <c r="B133" s="1">
         <v>0.95499999999999996</v>
@@ -2701,8 +2034,8 @@
       </c>
     </row>
     <row r="134" spans="1:3">
-      <c r="A134" s="1" t="s">
-        <v>110</v>
+      <c r="A134" s="2">
+        <v>44374</v>
       </c>
       <c r="B134" s="1">
         <v>0.873</v>
@@ -2712,8 +2045,8 @@
       </c>
     </row>
     <row r="135" spans="1:3">
-      <c r="A135" s="1" t="s">
-        <v>101</v>
+      <c r="A135" s="3">
+        <v>44375</v>
       </c>
       <c r="B135" s="1">
         <v>0.873</v>
@@ -2723,8 +2056,8 @@
       </c>
     </row>
     <row r="136" spans="1:3">
-      <c r="A136" s="1" t="s">
-        <v>95</v>
+      <c r="A136" s="2">
+        <v>44376</v>
       </c>
       <c r="B136" s="1">
         <v>0.873</v>
@@ -2734,8 +2067,8 @@
       </c>
     </row>
     <row r="137" spans="1:3">
-      <c r="A137" s="1" t="s">
-        <v>106</v>
+      <c r="A137" s="3">
+        <v>44377</v>
       </c>
       <c r="B137" s="1">
         <v>0.873</v>
@@ -2745,8 +2078,8 @@
       </c>
     </row>
     <row r="138" spans="1:3">
-      <c r="A138" s="1" t="s">
-        <v>99</v>
+      <c r="A138" s="2">
+        <v>44378</v>
       </c>
       <c r="B138" s="1">
         <v>0.873</v>
@@ -2756,8 +2089,8 @@
       </c>
     </row>
     <row r="139" spans="1:3">
-      <c r="A139" s="1" t="s">
-        <v>117</v>
+      <c r="A139" s="3">
+        <v>44379</v>
       </c>
       <c r="B139" s="1">
         <v>0.873</v>
@@ -2767,8 +2100,8 @@
       </c>
     </row>
     <row r="140" spans="1:3">
-      <c r="A140" s="1" t="s">
-        <v>98</v>
+      <c r="A140" s="2">
+        <v>44380</v>
       </c>
       <c r="B140" s="1">
         <v>0.873</v>
@@ -2778,8 +2111,8 @@
       </c>
     </row>
     <row r="141" spans="1:3">
-      <c r="A141" s="1" t="s">
-        <v>108</v>
+      <c r="A141" s="3">
+        <v>44381</v>
       </c>
       <c r="B141" s="1">
         <v>0.73499999999999999</v>
@@ -2789,8 +2122,8 @@
       </c>
     </row>
     <row r="142" spans="1:3">
-      <c r="A142" s="1" t="s">
-        <v>96</v>
+      <c r="A142" s="2">
+        <v>44382</v>
       </c>
       <c r="B142" s="1">
         <v>0.73499999999999999</v>
@@ -2800,8 +2133,8 @@
       </c>
     </row>
     <row r="143" spans="1:3">
-      <c r="A143" s="1" t="s">
-        <v>97</v>
+      <c r="A143" s="3">
+        <v>44383</v>
       </c>
       <c r="B143" s="1">
         <v>0.73499999999999999</v>
@@ -2811,8 +2144,8 @@
       </c>
     </row>
     <row r="144" spans="1:3">
-      <c r="A144" s="1" t="s">
-        <v>103</v>
+      <c r="A144" s="2">
+        <v>44384</v>
       </c>
       <c r="B144" s="1">
         <v>0.73499999999999999</v>
@@ -2822,8 +2155,8 @@
       </c>
     </row>
     <row r="145" spans="1:3">
-      <c r="A145" s="1" t="s">
-        <v>105</v>
+      <c r="A145" s="3">
+        <v>44385</v>
       </c>
       <c r="B145" s="1">
         <v>0.73499999999999999</v>
@@ -2833,8 +2166,8 @@
       </c>
     </row>
     <row r="146" spans="1:3">
-      <c r="A146" s="1" t="s">
-        <v>119</v>
+      <c r="A146" s="2">
+        <v>44386</v>
       </c>
       <c r="B146" s="1">
         <v>0.73499999999999999</v>
@@ -2844,8 +2177,8 @@
       </c>
     </row>
     <row r="147" spans="1:3">
-      <c r="A147" s="1" t="s">
-        <v>112</v>
+      <c r="A147" s="3">
+        <v>44387</v>
       </c>
       <c r="B147" s="1">
         <v>0.73499999999999999</v>
@@ -2855,8 +2188,8 @@
       </c>
     </row>
     <row r="148" spans="1:3">
-      <c r="A148" s="1" t="s">
-        <v>120</v>
+      <c r="A148" s="2">
+        <v>44388</v>
       </c>
       <c r="B148" s="1">
         <v>0.72278846153846155</v>
@@ -2866,8 +2199,8 @@
       </c>
     </row>
     <row r="149" spans="1:3">
-      <c r="A149" s="1" t="s">
-        <v>118</v>
+      <c r="A149" s="3">
+        <v>44389</v>
       </c>
       <c r="B149" s="1">
         <v>0.71057692307692311</v>
@@ -2877,8 +2210,8 @@
       </c>
     </row>
     <row r="150" spans="1:3">
-      <c r="A150" s="1" t="s">
-        <v>125</v>
+      <c r="A150" s="2">
+        <v>44390</v>
       </c>
       <c r="B150" s="1">
         <v>0.69836538461538467</v>
@@ -2888,8 +2221,8 @@
       </c>
     </row>
     <row r="151" spans="1:3">
-      <c r="A151" s="1" t="s">
-        <v>126</v>
+      <c r="A151" s="3">
+        <v>44391</v>
       </c>
       <c r="B151" s="1">
         <v>0.68615384615384623</v>
@@ -2899,8 +2232,8 @@
       </c>
     </row>
     <row r="152" spans="1:3">
-      <c r="A152" s="1" t="s">
-        <v>121</v>
+      <c r="A152" s="2">
+        <v>44392</v>
       </c>
       <c r="B152" s="1">
         <v>0.67394230769230778</v>
@@ -2910,8 +2243,8 @@
       </c>
     </row>
     <row r="153" spans="1:3">
-      <c r="A153" s="1" t="s">
-        <v>124</v>
+      <c r="A153" s="3">
+        <v>44393</v>
       </c>
       <c r="B153" s="1">
         <v>0.66173076923076934</v>
@@ -2921,8 +2254,8 @@
       </c>
     </row>
     <row r="154" spans="1:3">
-      <c r="A154" s="1" t="s">
-        <v>122</v>
+      <c r="A154" s="2">
+        <v>44394</v>
       </c>
       <c r="B154" s="1">
         <v>0.6495192307692309</v>
@@ -2932,8 +2265,8 @@
       </c>
     </row>
     <row r="155" spans="1:3">
-      <c r="A155" s="1" t="s">
-        <v>111</v>
+      <c r="A155" s="3">
+        <v>44395</v>
       </c>
       <c r="B155" s="1">
         <v>0.63730769230769246</v>
@@ -2943,8 +2276,8 @@
       </c>
     </row>
     <row r="156" spans="1:3">
-      <c r="A156" s="1" t="s">
-        <v>114</v>
+      <c r="A156" s="2">
+        <v>44396</v>
       </c>
       <c r="B156" s="1">
         <v>0.62509615384615402</v>
@@ -2954,8 +2287,8 @@
       </c>
     </row>
     <row r="157" spans="1:3">
-      <c r="A157" s="1" t="s">
-        <v>115</v>
+      <c r="A157" s="3">
+        <v>44397</v>
       </c>
       <c r="B157" s="1">
         <v>0.61288461538461558</v>
@@ -2965,8 +2298,8 @@
       </c>
     </row>
     <row r="158" spans="1:3">
-      <c r="A158" s="1" t="s">
-        <v>113</v>
+      <c r="A158" s="2">
+        <v>44398</v>
       </c>
       <c r="B158" s="1">
         <v>0.60067307692307714</v>
@@ -2976,8 +2309,8 @@
       </c>
     </row>
     <row r="159" spans="1:3">
-      <c r="A159" s="1" t="s">
-        <v>123</v>
+      <c r="A159" s="3">
+        <v>44399</v>
       </c>
       <c r="B159" s="1">
         <v>0.5884615384615387</v>
@@ -2987,8 +2320,8 @@
       </c>
     </row>
     <row r="160" spans="1:3">
-      <c r="A160" s="1" t="s">
-        <v>116</v>
+      <c r="A160" s="2">
+        <v>44400</v>
       </c>
       <c r="B160" s="1">
         <v>0.57625000000000026</v>
@@ -2998,8 +2331,8 @@
       </c>
     </row>
     <row r="161" spans="1:3">
-      <c r="A161" s="1" t="s">
-        <v>131</v>
+      <c r="A161" s="3">
+        <v>44401</v>
       </c>
       <c r="B161" s="1">
         <v>0.56403846153846182</v>
@@ -3009,8 +2342,8 @@
       </c>
     </row>
     <row r="162" spans="1:3">
-      <c r="A162" s="1" t="s">
-        <v>143</v>
+      <c r="A162" s="2">
+        <v>44402</v>
       </c>
       <c r="B162" s="1">
         <v>0.55182692307692338</v>
@@ -3020,8 +2353,8 @@
       </c>
     </row>
     <row r="163" spans="1:3">
-      <c r="A163" s="1" t="s">
-        <v>182</v>
+      <c r="A163" s="3">
+        <v>44403</v>
       </c>
       <c r="B163" s="1">
         <v>0.53961538461538494</v>
@@ -3031,8 +2364,8 @@
       </c>
     </row>
     <row r="164" spans="1:3">
-      <c r="A164" s="1" t="s">
-        <v>157</v>
+      <c r="A164" s="2">
+        <v>44404</v>
       </c>
       <c r="B164" s="1">
         <v>0.5274038461538465</v>
@@ -3042,8 +2375,8 @@
       </c>
     </row>
     <row r="165" spans="1:3">
-      <c r="A165" s="1" t="s">
-        <v>176</v>
+      <c r="A165" s="3">
+        <v>44405</v>
       </c>
       <c r="B165" s="1">
         <v>0.51519230769230806</v>
@@ -3053,8 +2386,8 @@
       </c>
     </row>
     <row r="166" spans="1:3">
-      <c r="A166" s="1" t="s">
-        <v>175</v>
+      <c r="A166" s="2">
+        <v>44406</v>
       </c>
       <c r="B166" s="1">
         <v>0.50298076923076962</v>
@@ -3064,8 +2397,8 @@
       </c>
     </row>
     <row r="167" spans="1:3">
-      <c r="A167" s="1" t="s">
-        <v>161</v>
+      <c r="A167" s="3">
+        <v>44407</v>
       </c>
       <c r="B167" s="1">
         <v>0.49076923076923118</v>
@@ -3075,8 +2408,8 @@
       </c>
     </row>
     <row r="168" spans="1:3">
-      <c r="A168" s="1" t="s">
-        <v>178</v>
+      <c r="A168" s="2">
+        <v>44408</v>
       </c>
       <c r="B168" s="1">
         <v>0.47855769230769274</v>
@@ -3086,8 +2419,8 @@
       </c>
     </row>
     <row r="169" spans="1:3">
-      <c r="A169" s="1" t="s">
-        <v>177</v>
+      <c r="A169" s="3">
+        <v>44409</v>
       </c>
       <c r="B169" s="1">
         <v>0.4663461538461543</v>
@@ -3097,8 +2430,8 @@
       </c>
     </row>
     <row r="170" spans="1:3">
-      <c r="A170" s="1" t="s">
-        <v>138</v>
+      <c r="A170" s="2">
+        <v>44410</v>
       </c>
       <c r="B170" s="1">
         <v>0.45413461538461586</v>
@@ -3108,8 +2441,8 @@
       </c>
     </row>
     <row r="171" spans="1:3">
-      <c r="A171" s="1" t="s">
-        <v>156</v>
+      <c r="A171" s="3">
+        <v>44411</v>
       </c>
       <c r="B171" s="1">
         <v>0.44192307692307742</v>
@@ -3119,8 +2452,8 @@
       </c>
     </row>
     <row r="172" spans="1:3">
-      <c r="A172" s="1" t="s">
-        <v>144</v>
+      <c r="A172" s="2">
+        <v>44412</v>
       </c>
       <c r="B172" s="1">
         <v>0.42971153846153898</v>
@@ -3130,8 +2463,8 @@
       </c>
     </row>
     <row r="173" spans="1:3">
-      <c r="A173" s="1" t="s">
-        <v>132</v>
+      <c r="A173" s="3">
+        <v>44413</v>
       </c>
       <c r="B173" s="1">
         <v>0.41750000000000054</v>
@@ -3141,8 +2474,8 @@
       </c>
     </row>
     <row r="174" spans="1:3">
-      <c r="A174" s="1" t="s">
-        <v>152</v>
+      <c r="A174" s="2">
+        <v>44414</v>
       </c>
       <c r="B174" s="1">
         <v>0.4052884615384621</v>
@@ -3152,8 +2485,8 @@
       </c>
     </row>
     <row r="175" spans="1:3">
-      <c r="A175" s="1" t="s">
-        <v>162</v>
+      <c r="A175" s="3">
+        <v>44415</v>
       </c>
       <c r="B175" s="1">
         <v>0.39307692307692366</v>
@@ -3163,8 +2496,8 @@
       </c>
     </row>
     <row r="176" spans="1:3">
-      <c r="A176" s="1" t="s">
-        <v>137</v>
+      <c r="A176" s="2">
+        <v>44416</v>
       </c>
       <c r="B176" s="1">
         <v>0.38086538461538522</v>
@@ -3174,8 +2507,8 @@
       </c>
     </row>
     <row r="177" spans="1:3">
-      <c r="A177" s="1" t="s">
-        <v>149</v>
+      <c r="A177" s="3">
+        <v>44417</v>
       </c>
       <c r="B177" s="1">
         <v>0.36865384615384678</v>
@@ -3185,8 +2518,8 @@
       </c>
     </row>
     <row r="178" spans="1:3">
-      <c r="A178" s="1" t="s">
-        <v>165</v>
+      <c r="A178" s="2">
+        <v>44418</v>
       </c>
       <c r="B178" s="1">
         <v>0.35644230769230834</v>
@@ -3196,8 +2529,8 @@
       </c>
     </row>
     <row r="179" spans="1:3">
-      <c r="A179" s="1" t="s">
-        <v>146</v>
+      <c r="A179" s="3">
+        <v>44419</v>
       </c>
       <c r="B179" s="1">
         <v>0.3442307692307699</v>
@@ -3207,8 +2540,8 @@
       </c>
     </row>
     <row r="180" spans="1:3">
-      <c r="A180" s="1" t="s">
-        <v>150</v>
+      <c r="A180" s="2">
+        <v>44420</v>
       </c>
       <c r="B180" s="1">
         <v>0.33201923076923145</v>
@@ -3218,8 +2551,8 @@
       </c>
     </row>
     <row r="181" spans="1:3">
-      <c r="A181" s="1" t="s">
-        <v>166</v>
+      <c r="A181" s="3">
+        <v>44421</v>
       </c>
       <c r="B181" s="1">
         <v>0.31980769230769301</v>
@@ -3229,8 +2562,8 @@
       </c>
     </row>
     <row r="182" spans="1:3">
-      <c r="A182" s="1" t="s">
-        <v>155</v>
+      <c r="A182" s="2">
+        <v>44422</v>
       </c>
       <c r="B182" s="1">
         <v>0.30759615384615457</v>
@@ -3240,8 +2573,8 @@
       </c>
     </row>
     <row r="183" spans="1:3">
-      <c r="A183" s="1" t="s">
-        <v>163</v>
+      <c r="A183" s="3">
+        <v>44423</v>
       </c>
       <c r="B183" s="1">
         <v>0.29538461538461613</v>
@@ -3251,8 +2584,8 @@
       </c>
     </row>
     <row r="184" spans="1:3">
-      <c r="A184" s="1" t="s">
-        <v>148</v>
+      <c r="A184" s="2">
+        <v>44424</v>
       </c>
       <c r="B184" s="1">
         <v>0.28317307692307769</v>
@@ -3262,8 +2595,8 @@
       </c>
     </row>
     <row r="185" spans="1:3">
-      <c r="A185" s="1" t="s">
-        <v>153</v>
+      <c r="A185" s="3">
+        <v>44425</v>
       </c>
       <c r="B185" s="1">
         <v>0.27096153846153925</v>
@@ -3273,8 +2606,8 @@
       </c>
     </row>
     <row r="186" spans="1:3">
-      <c r="A186" s="1" t="s">
-        <v>164</v>
+      <c r="A186" s="2">
+        <v>44426</v>
       </c>
       <c r="B186" s="1">
         <v>0.25875000000000081</v>
@@ -3284,8 +2617,8 @@
       </c>
     </row>
     <row r="187" spans="1:3">
-      <c r="A187" s="1" t="s">
-        <v>159</v>
+      <c r="A187" s="3">
+        <v>44427</v>
       </c>
       <c r="B187" s="1">
         <v>0.24653846153846237</v>
@@ -3295,8 +2628,8 @@
       </c>
     </row>
     <row r="188" spans="1:3">
-      <c r="A188" s="1" t="s">
-        <v>158</v>
+      <c r="A188" s="2">
+        <v>44428</v>
       </c>
       <c r="B188" s="1">
         <v>0.23432692307692393</v>
@@ -3306,8 +2639,8 @@
       </c>
     </row>
     <row r="189" spans="1:3">
-      <c r="A189" s="1" t="s">
-        <v>167</v>
+      <c r="A189" s="3">
+        <v>44429</v>
       </c>
       <c r="B189" s="1">
         <v>0.22211538461538549</v>
@@ -3317,8 +2650,8 @@
       </c>
     </row>
     <row r="190" spans="1:3">
-      <c r="A190" s="1" t="s">
-        <v>154</v>
+      <c r="A190" s="2">
+        <v>44430</v>
       </c>
       <c r="B190" s="1">
         <v>0.20990384615384705</v>
@@ -3328,8 +2661,8 @@
       </c>
     </row>
     <row r="191" spans="1:3">
-      <c r="A191" s="1" t="s">
-        <v>160</v>
+      <c r="A191" s="3">
+        <v>44431</v>
       </c>
       <c r="B191" s="1">
         <v>0.19769230769230861</v>
@@ -3339,8 +2672,8 @@
       </c>
     </row>
     <row r="192" spans="1:3">
-      <c r="A192" s="1" t="s">
-        <v>34</v>
+      <c r="A192" s="2">
+        <v>44432</v>
       </c>
       <c r="B192" s="1">
         <v>0.18548076923077017</v>
@@ -3350,8 +2683,8 @@
       </c>
     </row>
     <row r="193" spans="1:3">
-      <c r="A193" s="1" t="s">
-        <v>38</v>
+      <c r="A193" s="3">
+        <v>44433</v>
       </c>
       <c r="B193" s="1">
         <v>0.17326923076923173</v>
@@ -3361,8 +2694,8 @@
       </c>
     </row>
     <row r="194" spans="1:3">
-      <c r="A194" s="1" t="s">
-        <v>29</v>
+      <c r="A194" s="2">
+        <v>44434</v>
       </c>
       <c r="B194" s="1">
         <v>0.16105769230769329</v>
@@ -3372,8 +2705,8 @@
       </c>
     </row>
     <row r="195" spans="1:3">
-      <c r="A195" s="1" t="s">
-        <v>37</v>
+      <c r="A195" s="3">
+        <v>44435</v>
       </c>
       <c r="B195" s="1">
         <v>0.14884615384615485</v>
@@ -3383,8 +2716,8 @@
       </c>
     </row>
     <row r="196" spans="1:3">
-      <c r="A196" s="1" t="s">
-        <v>28</v>
+      <c r="A196" s="2">
+        <v>44436</v>
       </c>
       <c r="B196" s="1">
         <v>0.13663461538461641</v>
@@ -3394,8 +2727,8 @@
       </c>
     </row>
     <row r="197" spans="1:3">
-      <c r="A197" s="1" t="s">
-        <v>31</v>
+      <c r="A197" s="3">
+        <v>44437</v>
       </c>
       <c r="B197" s="1">
         <v>0.12442307692307797</v>
@@ -3405,8 +2738,8 @@
       </c>
     </row>
     <row r="198" spans="1:3">
-      <c r="A198" s="1" t="s">
-        <v>49</v>
+      <c r="A198" s="2">
+        <v>44438</v>
       </c>
       <c r="B198" s="1">
         <v>0.11221153846153953</v>
@@ -3416,8 +2749,8 @@
       </c>
     </row>
     <row r="199" spans="1:3">
-      <c r="A199" s="1" t="s">
-        <v>56</v>
+      <c r="A199" s="3">
+        <v>44439</v>
       </c>
       <c r="B199" s="1">
         <v>9.9999999999999978E-2</v>
@@ -3427,8 +2760,8 @@
       </c>
     </row>
     <row r="200" spans="1:3">
-      <c r="A200" s="1" t="s">
-        <v>43</v>
+      <c r="A200" s="2">
+        <v>44440</v>
       </c>
       <c r="B200" s="1">
         <v>9.9999999999999978E-2</v>
@@ -3438,8 +2771,8 @@
       </c>
     </row>
     <row r="201" spans="1:3">
-      <c r="A201" s="1" t="s">
-        <v>139</v>
+      <c r="A201" s="3">
+        <v>44441</v>
       </c>
       <c r="B201" s="1">
         <v>9.9999999999999978E-2</v>
@@ -3449,8 +2782,8 @@
       </c>
     </row>
     <row r="202" spans="1:3">
-      <c r="A202" s="1" t="s">
-        <v>140</v>
+      <c r="A202" s="2">
+        <v>44442</v>
       </c>
       <c r="B202" s="1">
         <v>9.9999999999999978E-2</v>
@@ -3460,8 +2793,8 @@
       </c>
     </row>
     <row r="203" spans="1:3">
-      <c r="A203" s="1" t="s">
-        <v>151</v>
+      <c r="A203" s="3">
+        <v>44443</v>
       </c>
       <c r="B203" s="1">
         <v>9.9999999999999978E-2</v>
@@ -3471,8 +2804,8 @@
       </c>
     </row>
     <row r="204" spans="1:3">
-      <c r="A204" s="1" t="s">
-        <v>60</v>
+      <c r="A204" s="2">
+        <v>44444</v>
       </c>
       <c r="B204" s="1">
         <v>9.9999999999999978E-2</v>
@@ -3482,8 +2815,8 @@
       </c>
     </row>
     <row r="205" spans="1:3">
-      <c r="A205" s="1" t="s">
-        <v>66</v>
+      <c r="A205" s="3">
+        <v>44445</v>
       </c>
       <c r="B205" s="1">
         <v>9.9999999999999978E-2</v>
@@ -3493,8 +2826,8 @@
       </c>
     </row>
     <row r="206" spans="1:3">
-      <c r="A206" s="1" t="s">
-        <v>62</v>
+      <c r="A206" s="2">
+        <v>44446</v>
       </c>
       <c r="B206" s="1">
         <v>9.9999999999999978E-2</v>
@@ -3504,8 +2837,8 @@
       </c>
     </row>
     <row r="207" spans="1:3">
-      <c r="A207" s="1" t="s">
-        <v>61</v>
+      <c r="A207" s="3">
+        <v>44447</v>
       </c>
       <c r="B207" s="1">
         <v>9.9999999999999978E-2</v>
@@ -3515,8 +2848,8 @@
       </c>
     </row>
     <row r="208" spans="1:3">
-      <c r="A208" s="1" t="s">
-        <v>65</v>
+      <c r="A208" s="2">
+        <v>44448</v>
       </c>
       <c r="B208" s="1">
         <v>9.9999999999999978E-2</v>
@@ -3526,8 +2859,8 @@
       </c>
     </row>
     <row r="209" spans="1:3">
-      <c r="A209" s="1" t="s">
-        <v>142</v>
+      <c r="A209" s="3">
+        <v>44449</v>
       </c>
       <c r="B209" s="1">
         <v>9.9999999999999978E-2</v>
@@ -3537,8 +2870,8 @@
       </c>
     </row>
     <row r="210" spans="1:3">
-      <c r="A210" s="1" t="s">
-        <v>147</v>
+      <c r="A210" s="2">
+        <v>44450</v>
       </c>
       <c r="B210" s="1">
         <v>9.9999999999999978E-2</v>
@@ -3548,8 +2881,8 @@
       </c>
     </row>
     <row r="211" spans="1:3">
-      <c r="A211" s="1" t="s">
-        <v>136</v>
+      <c r="A211" s="3">
+        <v>44451</v>
       </c>
       <c r="B211" s="1">
         <v>9.9999999999999978E-2</v>
@@ -3559,8 +2892,8 @@
       </c>
     </row>
     <row r="212" spans="1:3">
-      <c r="A212" s="1" t="s">
-        <v>134</v>
+      <c r="A212" s="2">
+        <v>44452</v>
       </c>
       <c r="B212" s="1">
         <v>9.9999999999999978E-2</v>
@@ -3570,8 +2903,8 @@
       </c>
     </row>
     <row r="213" spans="1:3">
-      <c r="A213" s="1" t="s">
-        <v>141</v>
+      <c r="A213" s="3">
+        <v>44453</v>
       </c>
       <c r="B213" s="1">
         <v>9.9999999999999978E-2</v>
@@ -3581,8 +2914,8 @@
       </c>
     </row>
     <row r="214" spans="1:3">
-      <c r="A214" s="1" t="s">
-        <v>135</v>
+      <c r="A214" s="2">
+        <v>44454</v>
       </c>
       <c r="B214" s="1">
         <v>9.9999999999999978E-2</v>
@@ -3592,8 +2925,8 @@
       </c>
     </row>
     <row r="215" spans="1:3">
-      <c r="A215" s="1" t="s">
-        <v>133</v>
+      <c r="A215" s="3">
+        <v>44455</v>
       </c>
       <c r="B215" s="1">
         <v>9.9999999999999978E-2</v>
@@ -3603,8 +2936,8 @@
       </c>
     </row>
     <row r="216" spans="1:3">
-      <c r="A216" s="1" t="s">
-        <v>48</v>
+      <c r="A216" s="2">
+        <v>44456</v>
       </c>
       <c r="B216" s="1">
         <v>9.9999999999999978E-2</v>
@@ -3614,8 +2947,8 @@
       </c>
     </row>
     <row r="217" spans="1:3">
-      <c r="A217" s="1" t="s">
-        <v>53</v>
+      <c r="A217" s="3">
+        <v>44457</v>
       </c>
       <c r="B217" s="1">
         <v>9.9999999999999978E-2</v>
@@ -3625,8 +2958,8 @@
       </c>
     </row>
     <row r="218" spans="1:3">
-      <c r="A218" s="1" t="s">
-        <v>67</v>
+      <c r="A218" s="2">
+        <v>44458</v>
       </c>
       <c r="B218" s="1">
         <v>9.9999999999999978E-2</v>
@@ -3636,8 +2969,8 @@
       </c>
     </row>
     <row r="219" spans="1:3">
-      <c r="A219" s="1" t="s">
-        <v>58</v>
+      <c r="A219" s="3">
+        <v>44459</v>
       </c>
       <c r="B219" s="1">
         <v>9.9999999999999978E-2</v>
@@ -3647,8 +2980,8 @@
       </c>
     </row>
     <row r="220" spans="1:3">
-      <c r="A220" s="1" t="s">
-        <v>51</v>
+      <c r="A220" s="2">
+        <v>44460</v>
       </c>
       <c r="B220" s="1">
         <v>9.9999999999999978E-2</v>
@@ -3658,8 +2991,8 @@
       </c>
     </row>
     <row r="221" spans="1:3">
-      <c r="A221" s="1" t="s">
-        <v>45</v>
+      <c r="A221" s="3">
+        <v>44461</v>
       </c>
       <c r="B221" s="1">
         <v>9.9999999999999978E-2</v>
@@ -3669,8 +3002,8 @@
       </c>
     </row>
     <row r="222" spans="1:3">
-      <c r="A222" s="1" t="s">
-        <v>59</v>
+      <c r="A222" s="2">
+        <v>44462</v>
       </c>
       <c r="B222" s="1">
         <v>9.9999999999999978E-2</v>
@@ -3680,8 +3013,8 @@
       </c>
     </row>
     <row r="223" spans="1:3">
-      <c r="A223" s="1" t="s">
-        <v>57</v>
+      <c r="A223" s="3">
+        <v>44463</v>
       </c>
       <c r="B223" s="1">
         <v>9.9999999999999978E-2</v>
@@ -3691,8 +3024,8 @@
       </c>
     </row>
     <row r="224" spans="1:3">
-      <c r="A224" s="1" t="s">
-        <v>54</v>
+      <c r="A224" s="2">
+        <v>44464</v>
       </c>
       <c r="B224" s="1">
         <v>9.9999999999999978E-2</v>
@@ -3702,8 +3035,8 @@
       </c>
     </row>
     <row r="225" spans="1:3">
-      <c r="A225" s="1" t="s">
-        <v>46</v>
+      <c r="A225" s="3">
+        <v>44465</v>
       </c>
       <c r="B225" s="1">
         <v>9.9999999999999978E-2</v>
@@ -3713,8 +3046,8 @@
       </c>
     </row>
     <row r="226" spans="1:3">
-      <c r="A226" s="1" t="s">
-        <v>44</v>
+      <c r="A226" s="2">
+        <v>44466</v>
       </c>
       <c r="B226" s="1">
         <v>9.9999999999999978E-2</v>
@@ -3724,8 +3057,8 @@
       </c>
     </row>
     <row r="227" spans="1:3">
-      <c r="A227" s="1" t="s">
-        <v>50</v>
+      <c r="A227" s="3">
+        <v>44467</v>
       </c>
       <c r="B227" s="1">
         <v>9.9999999999999978E-2</v>
@@ -3735,8 +3068,8 @@
       </c>
     </row>
     <row r="228" spans="1:3">
-      <c r="A228" s="1" t="s">
-        <v>63</v>
+      <c r="A228" s="2">
+        <v>44468</v>
       </c>
       <c r="B228" s="1">
         <v>9.9999999999999978E-2</v>
@@ -3746,8 +3079,8 @@
       </c>
     </row>
     <row r="229" spans="1:3">
-      <c r="A229" s="1" t="s">
-        <v>145</v>
+      <c r="A229" s="2">
+        <v>44469</v>
       </c>
       <c r="B229" s="1">
         <v>0.1</v>
@@ -3756,7 +3089,1020 @@
         <v>0.9</v>
       </c>
     </row>
+    <row r="230" spans="1:3">
+      <c r="A230" s="2">
+        <v>44470</v>
+      </c>
+      <c r="B230" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C230" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3">
+      <c r="A231" s="2">
+        <v>44471</v>
+      </c>
+      <c r="B231" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C231" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3">
+      <c r="A232" s="2">
+        <v>44472</v>
+      </c>
+      <c r="B232" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C232" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3">
+      <c r="A233" s="2">
+        <v>44473</v>
+      </c>
+      <c r="B233" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C233" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3">
+      <c r="A234" s="2">
+        <v>44474</v>
+      </c>
+      <c r="B234" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C234" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3">
+      <c r="A235" s="2">
+        <v>44475</v>
+      </c>
+      <c r="B235" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C235" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3">
+      <c r="A236" s="2">
+        <v>44476</v>
+      </c>
+      <c r="B236" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C236" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3">
+      <c r="A237" s="2">
+        <v>44477</v>
+      </c>
+      <c r="B237" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C237" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3">
+      <c r="A238" s="2">
+        <v>44478</v>
+      </c>
+      <c r="B238" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C238" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3">
+      <c r="A239" s="2">
+        <v>44479</v>
+      </c>
+      <c r="B239" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C239" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3">
+      <c r="A240" s="2">
+        <v>44480</v>
+      </c>
+      <c r="B240" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C240" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3">
+      <c r="A241" s="2">
+        <v>44481</v>
+      </c>
+      <c r="B241" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C241" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3">
+      <c r="A242" s="2">
+        <v>44482</v>
+      </c>
+      <c r="B242" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C242" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3">
+      <c r="A243" s="2">
+        <v>44483</v>
+      </c>
+      <c r="B243" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C243" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3">
+      <c r="A244" s="2">
+        <v>44484</v>
+      </c>
+      <c r="B244" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C244" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3">
+      <c r="A245" s="2">
+        <v>44485</v>
+      </c>
+      <c r="B245" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C245" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3">
+      <c r="A246" s="2">
+        <v>44486</v>
+      </c>
+      <c r="B246" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C246" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3">
+      <c r="A247" s="2">
+        <v>44487</v>
+      </c>
+      <c r="B247" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C247" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3">
+      <c r="A248" s="2">
+        <v>44488</v>
+      </c>
+      <c r="B248" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C248" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3">
+      <c r="A249" s="2">
+        <v>44489</v>
+      </c>
+      <c r="B249" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C249" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3">
+      <c r="A250" s="2">
+        <v>44490</v>
+      </c>
+      <c r="B250" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C250" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3">
+      <c r="A251" s="2">
+        <v>44491</v>
+      </c>
+      <c r="B251" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C251" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3">
+      <c r="A252" s="2">
+        <v>44492</v>
+      </c>
+      <c r="B252" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C252" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3">
+      <c r="A253" s="2">
+        <v>44493</v>
+      </c>
+      <c r="B253" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C253" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3">
+      <c r="A254" s="2">
+        <v>44494</v>
+      </c>
+      <c r="B254" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C254" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3">
+      <c r="A255" s="2">
+        <v>44495</v>
+      </c>
+      <c r="B255" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C255" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3">
+      <c r="A256" s="2">
+        <v>44496</v>
+      </c>
+      <c r="B256" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C256" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3">
+      <c r="A257" s="2">
+        <v>44497</v>
+      </c>
+      <c r="B257" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C257" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3">
+      <c r="A258" s="2">
+        <v>44498</v>
+      </c>
+      <c r="B258" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C258" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3">
+      <c r="A259" s="2">
+        <v>44499</v>
+      </c>
+      <c r="B259" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C259" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3">
+      <c r="A260" s="2">
+        <v>44500</v>
+      </c>
+      <c r="B260" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C260" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3">
+      <c r="A261" s="2">
+        <v>44501</v>
+      </c>
+      <c r="B261" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C261" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3">
+      <c r="A262" s="2">
+        <v>44502</v>
+      </c>
+      <c r="B262" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C262" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3">
+      <c r="A263" s="2">
+        <v>44503</v>
+      </c>
+      <c r="B263" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C263" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3">
+      <c r="A264" s="2">
+        <v>44504</v>
+      </c>
+      <c r="B264" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C264" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3">
+      <c r="A265" s="2">
+        <v>44505</v>
+      </c>
+      <c r="B265" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C265" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3">
+      <c r="A266" s="2">
+        <v>44506</v>
+      </c>
+      <c r="B266" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C266" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3">
+      <c r="A267" s="2">
+        <v>44507</v>
+      </c>
+      <c r="B267" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C267" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3">
+      <c r="A268" s="2">
+        <v>44508</v>
+      </c>
+      <c r="B268" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C268" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3">
+      <c r="A269" s="2">
+        <v>44509</v>
+      </c>
+      <c r="B269" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C269" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3">
+      <c r="A270" s="2">
+        <v>44510</v>
+      </c>
+      <c r="B270" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C270" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3">
+      <c r="A271" s="2">
+        <v>44511</v>
+      </c>
+      <c r="B271" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C271" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3">
+      <c r="A272" s="2">
+        <v>44512</v>
+      </c>
+      <c r="B272" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C272" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3">
+      <c r="A273" s="2">
+        <v>44513</v>
+      </c>
+      <c r="B273" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C273" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3">
+      <c r="A274" s="2">
+        <v>44514</v>
+      </c>
+      <c r="B274" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C274" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3">
+      <c r="A275" s="2">
+        <v>44515</v>
+      </c>
+      <c r="B275" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C275" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3">
+      <c r="A276" s="2">
+        <v>44516</v>
+      </c>
+      <c r="B276" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C276" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3">
+      <c r="A277" s="2">
+        <v>44517</v>
+      </c>
+      <c r="B277" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C277" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3">
+      <c r="A278" s="2">
+        <v>44518</v>
+      </c>
+      <c r="B278" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C278" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3">
+      <c r="A279" s="2">
+        <v>44519</v>
+      </c>
+      <c r="B279" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C279" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3">
+      <c r="A280" s="2">
+        <v>44520</v>
+      </c>
+      <c r="B280" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C280" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3">
+      <c r="A281" s="2">
+        <v>44521</v>
+      </c>
+      <c r="B281" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C281" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3">
+      <c r="A282" s="2">
+        <v>44522</v>
+      </c>
+      <c r="B282" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C282" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3">
+      <c r="A283" s="2">
+        <v>44523</v>
+      </c>
+      <c r="B283" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C283" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3">
+      <c r="A284" s="2">
+        <v>44524</v>
+      </c>
+      <c r="B284" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C284" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3">
+      <c r="A285" s="2">
+        <v>44525</v>
+      </c>
+      <c r="B285" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C285" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3">
+      <c r="A286" s="2">
+        <v>44526</v>
+      </c>
+      <c r="B286" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C286" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3">
+      <c r="A287" s="2">
+        <v>44527</v>
+      </c>
+      <c r="B287" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C287" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3">
+      <c r="A288" s="2">
+        <v>44528</v>
+      </c>
+      <c r="B288" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C288" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3">
+      <c r="A289" s="2">
+        <v>44529</v>
+      </c>
+      <c r="B289" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C289" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3">
+      <c r="A290" s="2">
+        <v>44530</v>
+      </c>
+      <c r="B290" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C290" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3">
+      <c r="A291" s="2">
+        <v>44531</v>
+      </c>
+      <c r="B291" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C291" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3">
+      <c r="A292" s="2">
+        <v>44532</v>
+      </c>
+      <c r="B292" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C292" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3">
+      <c r="A293" s="2">
+        <v>44533</v>
+      </c>
+      <c r="B293" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C293" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3">
+      <c r="A294" s="2">
+        <v>44534</v>
+      </c>
+      <c r="B294" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C294" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3">
+      <c r="A295" s="2">
+        <v>44535</v>
+      </c>
+      <c r="B295" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C295" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3">
+      <c r="A296" s="2">
+        <v>44536</v>
+      </c>
+      <c r="B296" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C296" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3">
+      <c r="A297" s="2">
+        <v>44537</v>
+      </c>
+      <c r="B297" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C297" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3">
+      <c r="A298" s="2">
+        <v>44538</v>
+      </c>
+      <c r="B298" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C298" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3">
+      <c r="A299" s="2">
+        <v>44539</v>
+      </c>
+      <c r="B299" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C299" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3">
+      <c r="A300" s="2">
+        <v>44540</v>
+      </c>
+      <c r="B300" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C300" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3">
+      <c r="A301" s="2">
+        <v>44541</v>
+      </c>
+      <c r="B301" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C301" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3">
+      <c r="A302" s="2">
+        <v>44542</v>
+      </c>
+      <c r="B302" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C302" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3">
+      <c r="A303" s="2">
+        <v>44543</v>
+      </c>
+      <c r="B303" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C303" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="304" spans="1:3">
+      <c r="A304" s="2">
+        <v>44544</v>
+      </c>
+      <c r="B304" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C304" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="305" spans="1:3">
+      <c r="A305" s="2">
+        <v>44545</v>
+      </c>
+      <c r="B305" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C305" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="306" spans="1:3">
+      <c r="A306" s="2">
+        <v>44546</v>
+      </c>
+      <c r="B306" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C306" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="307" spans="1:3">
+      <c r="A307" s="2">
+        <v>44547</v>
+      </c>
+      <c r="B307" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C307" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="308" spans="1:3">
+      <c r="A308" s="2">
+        <v>44548</v>
+      </c>
+      <c r="B308" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C308" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="309" spans="1:3">
+      <c r="A309" s="2">
+        <v>44549</v>
+      </c>
+      <c r="B309" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C309" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="310" spans="1:3">
+      <c r="A310" s="2">
+        <v>44550</v>
+      </c>
+      <c r="B310" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C310" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="311" spans="1:3">
+      <c r="A311" s="2">
+        <v>44551</v>
+      </c>
+      <c r="B311" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C311" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="312" spans="1:3">
+      <c r="A312" s="2">
+        <v>44552</v>
+      </c>
+      <c r="B312" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C312" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="313" spans="1:3">
+      <c r="A313" s="2">
+        <v>44553</v>
+      </c>
+      <c r="B313" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C313" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="314" spans="1:3">
+      <c r="A314" s="2">
+        <v>44554</v>
+      </c>
+      <c r="B314" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C314" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="315" spans="1:3">
+      <c r="A315" s="2">
+        <v>44555</v>
+      </c>
+      <c r="B315" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C315" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="316" spans="1:3">
+      <c r="A316" s="2">
+        <v>44556</v>
+      </c>
+      <c r="B316" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C316" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="317" spans="1:3">
+      <c r="A317" s="2">
+        <v>44557</v>
+      </c>
+      <c r="B317" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C317" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="318" spans="1:3">
+      <c r="A318" s="2">
+        <v>44558</v>
+      </c>
+      <c r="B318" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C318" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="319" spans="1:3">
+      <c r="A319" s="2">
+        <v>44559</v>
+      </c>
+      <c r="B319" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C319" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="320" spans="1:3">
+      <c r="A320" s="2">
+        <v>44560</v>
+      </c>
+      <c r="B320" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C320" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="321" spans="1:3">
+      <c r="A321" s="2">
+        <v>44561</v>
+      </c>
+      <c r="B321" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C321" s="1">
+        <v>0.9</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.74805557727813721" right="0.74805557727813721" top="0.98430556058883667" bottom="0.98430556058883667" header="0.51152777671813965" footer="0.51152777671813965"/>
   <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait"/>
 </worksheet>

</xml_diff>